<commit_message>
Removed labs keeping tuts
</commit_message>
<xml_diff>
--- a/A4 - Time tables/csvs/Temp.xlsx
+++ b/A4 - Time tables/csvs/Temp.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="185">
   <si>
     <t xml:space="preserve">Room</t>
   </si>
@@ -59,6 +59,9 @@
     <t xml:space="preserve">A1</t>
   </si>
   <si>
+    <t xml:space="preserve">K</t>
+  </si>
+  <si>
     <t xml:space="preserve">EE230</t>
   </si>
   <si>
@@ -296,201 +299,201 @@
     <t xml:space="preserve">PH706</t>
   </si>
   <si>
+    <t xml:space="preserve">PH516</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME615</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME618</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME321M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME324</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME619</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1G2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME522</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME686</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME513</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME691</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME514</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME662</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME532</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME613</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1G1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xxxx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE270</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE533</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE385</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE580</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE673</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE504</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE514</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE649</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE524</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE661</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE556</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE533</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE594</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT514</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS623</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH704</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH527</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH543</t>
+  </si>
+  <si>
     <t xml:space="preserve">PH412</t>
   </si>
   <si>
-    <t xml:space="preserve">PH516</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME615</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME223</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME224</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME618</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME321M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME324</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME322</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME688</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME619</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1G2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME522</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME686</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME513</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME691</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME514</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME662</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME532</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME613</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1G1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME421</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xxxx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME695</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EE626</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EE270</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EE337</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EE533</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EE385</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EE333</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EE625</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EE580</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EE551</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EE673</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CE201</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CE222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CE309</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CE304</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CE504</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CE514</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CE649</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CE524</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CE661</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CE556</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CE533</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CE594</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT514</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS623</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS502</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS505</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH308</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH408</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH704</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH527</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH543</t>
-  </si>
-  <si>
     <t xml:space="preserve">PH521</t>
   </si>
   <si>
@@ -518,9 +521,6 @@
     <t xml:space="preserve">ME326</t>
   </si>
   <si>
-    <t xml:space="preserve">CL309</t>
-  </si>
-  <si>
     <t xml:space="preserve">EE647</t>
   </si>
   <si>
@@ -576,9 +576,6 @@
   </si>
   <si>
     <t xml:space="preserve">ME670</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I</t>
   </si>
   <si>
     <t xml:space="preserve">CE402</t>
@@ -678,10 +675,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -724,28 +721,31 @@
       <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>2002</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -753,25 +753,25 @@
         <v>2201</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -779,16 +779,16 @@
         <v>2202</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -796,22 +796,22 @@
         <v>3101</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -819,19 +819,19 @@
         <v>4101</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -839,7 +839,7 @@
         <v>3202</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -847,7 +847,7 @@
         <v>2101</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -855,22 +855,22 @@
         <v>4201</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,25 +878,25 @@
         <v>3102</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -904,25 +904,25 @@
         <v>4208</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -930,16 +930,16 @@
         <v>4205</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,18 +947,18 @@
         <v>4211</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -966,7 +966,7 @@
         <v>4001</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,16 +974,16 @@
         <v>1206</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -991,16 +991,16 @@
         <v>1101</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1008,10 +1008,10 @@
         <v>1102</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1019,13 +1019,13 @@
         <v>4206</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1033,16 +1033,16 @@
         <v>4003</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1050,22 +1050,22 @@
         <v>4004</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1073,10 +1073,10 @@
         <v>4212</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,18 +1084,9 @@
         <v>4004</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="J23" s="0" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1103,16 +1094,7 @@
       <c r="A24" s="0" t="n">
         <v>4212</v>
       </c>
-      <c r="H24" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="K24" s="0" t="s">
+      <c r="L24" s="0" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1254,17 +1236,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G36" activeCellId="0" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="2.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
@@ -1310,13 +1292,13 @@
         <v>2002</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1330,16 +1312,16 @@
         <v>122</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>123</v>
@@ -1350,13 +1332,13 @@
         <v>2202</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="E4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>124</v>
@@ -1373,13 +1355,13 @@
         <v>126</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J5" s="0" t="s">
         <v>127</v>
@@ -1396,10 +1378,10 @@
         <v>129</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J6" s="0" t="s">
         <v>130</v>
@@ -1410,7 +1392,7 @@
         <v>3202</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1418,7 +1400,7 @@
         <v>2101</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1429,16 +1411,16 @@
         <v>131</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>132</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>133</v>
@@ -1447,7 +1429,7 @@
         <v>134</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1458,16 +1440,16 @@
         <v>135</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J10" s="0" t="s">
         <v>136</v>
@@ -1484,7 +1466,7 @@
         <v>138</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>139</v>
@@ -1493,10 +1475,10 @@
         <v>139</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J11" s="0" t="s">
         <v>140</v>
@@ -1510,13 +1492,13 @@
         <v>141</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1524,13 +1506,13 @@
         <v>4211</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J13" s="0" t="s">
         <v>142</v>
@@ -1538,10 +1520,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1549,7 +1531,7 @@
         <v>4001</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1563,7 +1545,7 @@
         <v>143</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1577,10 +1559,10 @@
         <v>145</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1591,7 +1573,7 @@
         <v>146</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1602,10 +1584,10 @@
         <v>147</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1619,10 +1601,10 @@
         <v>149</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1633,7 +1615,7 @@
         <v>150</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>151</v>
@@ -1642,7 +1624,7 @@
         <v>152</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1653,19 +1635,19 @@
         <v>153</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>154</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>90</v>
+        <v>155</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>90</v>
+        <v>155</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>90</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,16 +1655,16 @@
         <v>4004</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1693,7 +1675,7 @@
         <v>92</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>93</v>
@@ -1711,7 +1693,7 @@
         <v>101</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1722,7 +1704,7 @@
         <v>102</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>93</v>
@@ -1731,7 +1713,7 @@
         <v>94</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H25" s="0" t="s">
         <v>99</v>
@@ -1743,7 +1725,7 @@
         <v>101</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1779,7 +1761,7 @@
         <v>111</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,20 +1777,12 @@
         <v>116</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
-        <v>4203</v>
-      </c>
-      <c r="L31" s="0" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1828,10 +1802,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1877,19 +1851,22 @@
       <c r="K1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>2002</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>16</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>165</v>
@@ -1908,22 +1885,22 @@
         <v>2201</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>168</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>123</v>
@@ -1934,10 +1911,10 @@
         <v>2202</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>124</v>
@@ -1954,13 +1931,13 @@
         <v>3101</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>127</v>
@@ -1971,10 +1948,10 @@
         <v>4101</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>130</v>
@@ -1994,13 +1971,13 @@
         <v>131</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K8" s="0" t="s">
         <v>133</v>
@@ -2017,10 +1994,10 @@
         <v>135</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>136</v>
@@ -2037,16 +2014,16 @@
         <v>138</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>140</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2054,16 +2031,16 @@
         <v>4205</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>141</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2071,13 +2048,13 @@
         <v>4211</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>134</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>142</v>
@@ -2088,16 +2065,16 @@
         <v>1206</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H13" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="I13" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="J13" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2108,7 +2085,7 @@
         <v>145</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2116,7 +2093,7 @@
         <v>1102</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>173</v>
@@ -2125,7 +2102,7 @@
         <v>146</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,10 +2110,10 @@
         <v>4206</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>147</v>
@@ -2150,16 +2127,16 @@
         <v>149</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>148</v>
       </c>
       <c r="H17" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="0" t="s">
         <v>80</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>79</v>
       </c>
       <c r="J17" s="0" t="s">
         <v>174</v>
@@ -2170,28 +2147,28 @@
         <v>4004</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>151</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>152</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2199,7 +2176,7 @@
         <v>4212</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>175</v>
@@ -2208,18 +2185,9 @@
         <v>153</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="K19" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="L19" s="0" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2227,16 +2195,7 @@
       <c r="A20" s="0" t="n">
         <v>4003</v>
       </c>
-      <c r="H20" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="K20" s="0" t="s">
+      <c r="L20" s="0" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2251,7 +2210,7 @@
         <v>96</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>93</v>
@@ -2263,7 +2222,7 @@
         <v>97</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K21" s="0" t="s">
         <v>98</v>
@@ -2277,7 +2236,7 @@
         <v>102</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>93</v>
@@ -2286,7 +2245,7 @@
         <v>178</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K22" s="0" t="s">
         <v>98</v>
@@ -2372,17 +2331,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="2.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
@@ -2423,7 +2382,7 @@
         <v>8</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>184</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2431,13 +2390,13 @@
         <v>2002</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>165</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2456,7 +2415,7 @@
         <v>121</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>122</v>
@@ -2476,7 +2435,7 @@
         <v>129</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>125</v>
@@ -2485,7 +2444,7 @@
         <v>169</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2499,7 +2458,7 @@
         <v>127</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2510,7 +2469,7 @@
         <v>128</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>170</v>
@@ -2524,7 +2483,7 @@
         <v>4201</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>171</v>
@@ -2539,7 +2498,7 @@
         <v>134</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J8" s="0" t="s">
         <v>133</v>
@@ -2550,7 +2509,7 @@
         <v>3102</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>172</v>
@@ -2559,7 +2518,7 @@
         <v>135</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>136</v>
@@ -2568,7 +2527,7 @@
         <v>137</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2576,7 +2535,7 @@
         <v>4208</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>138</v>
@@ -2593,13 +2552,13 @@
         <v>4205</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>141</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2607,7 +2566,7 @@
         <v>4211</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>142</v>
@@ -2621,10 +2580,10 @@
         <v>143</v>
       </c>
       <c r="H14" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2632,10 +2591,10 @@
         <v>1101</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>145</v>
@@ -2663,10 +2622,10 @@
         <v>147</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2674,10 +2633,10 @@
         <v>4003</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>77</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>149</v>
@@ -2686,7 +2645,7 @@
         <v>174</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2697,19 +2656,19 @@
         <v>151</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>150</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2723,38 +2682,29 @@
         <v>175</v>
       </c>
       <c r="D20" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>87</v>
-      </c>
       <c r="H20" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I20" s="0" t="s">
         <v>154</v>
       </c>
       <c r="J20" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="K20" s="0" t="s">
         <v>158</v>
-      </c>
-      <c r="K20" s="0" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>4003</v>
       </c>
-      <c r="H21" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="K21" s="0" t="s">
+      <c r="L21" s="0" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2769,7 +2719,7 @@
         <v>95</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>177</v>
@@ -2778,7 +2728,7 @@
         <v>101</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J22" s="0" t="s">
         <v>98</v>
@@ -2798,10 +2748,10 @@
         <v>95</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>178</v>
@@ -2810,7 +2760,7 @@
         <v>101</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J23" s="0" t="s">
         <v>98</v>
@@ -2855,7 +2805,7 @@
         <v>111</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>181</v>
@@ -2875,14 +2825,6 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
-        <v>4203</v>
-      </c>
-      <c r="L29" s="0" t="s">
-        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2904,7 +2846,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2957,19 +2899,19 @@
         <v>2002</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>165</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2991,16 +2933,16 @@
         <v>122</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>168</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3008,7 +2950,7 @@
         <v>2202</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>124</v>
@@ -3017,7 +2959,7 @@
         <v>169</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3028,13 +2970,13 @@
         <v>126</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3051,10 +2993,10 @@
         <v>170</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3062,7 +3004,7 @@
         <v>3202</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3070,7 +3012,7 @@
         <v>2101</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3081,10 +3023,10 @@
         <v>132</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>171</v>
@@ -3093,7 +3035,7 @@
         <v>133</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3101,25 +3043,25 @@
         <v>3102</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>172</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3130,16 +3072,16 @@
         <v>139</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>138</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3147,7 +3089,7 @@
         <v>4205</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>141</v>
@@ -3158,15 +3100,15 @@
         <v>4211</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3174,7 +3116,7 @@
         <v>4001</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3182,7 +3124,7 @@
         <v>1206</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3190,16 +3132,16 @@
         <v>1101</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>144</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3210,7 +3152,7 @@
         <v>173</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3218,10 +3160,10 @@
         <v>4206</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3243,25 +3185,25 @@
         <v>4004</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>81</v>
-      </c>
       <c r="G22" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>152</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3269,19 +3211,19 @@
         <v>4212</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>175</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H23" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="I23" s="0" t="s">
         <v>158</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>157</v>
       </c>
       <c r="J23" s="0" t="s">
         <v>154</v>
@@ -3337,7 +3279,7 @@
         <v>104</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K27" s="0" t="s">
         <v>105</v>
@@ -3359,7 +3301,7 @@
         <v>1203</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>181</v>

</xml_diff>